<commit_message>
Add Yuewen Ma x24134511's work of wasm;
</commit_message>
<xml_diff>
--- a/Web Assembly - 4th Week/Web Assembly.xlsx
+++ b/Web Assembly - 4th Week/Web Assembly.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NCI\Foundations of AI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-repos\NCI-Foundations-of-AI-Weekly-Tasks\Web Assembly - 4th Week\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322F7B2B-760C-4497-B1E2-9480A69EC384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D7792A-ABD6-420D-87CB-4D61817B2E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{B6BF587D-12F9-4973-87CD-6C0886494E04}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6BF587D-12F9-4973-87CD-6C0886494E04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -79,18 +79,33 @@
   </si>
   <si>
     <t>Submitted in Git Repo</t>
+  </si>
+  <si>
+    <t>Yuewen Ma</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Python, Java, Go</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -135,12 +150,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -161,9 +179,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -201,7 +219,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -307,7 +325,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -449,7 +467,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -457,20 +475,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8484C3E4-72CF-4A08-A46B-0A4FCF1A79AA}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,7 +499,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -492,7 +510,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -503,7 +521,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -514,7 +532,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -525,7 +543,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -536,7 +554,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -547,7 +565,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -558,7 +576,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -569,7 +587,19 @@
         <v>17</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>